<commit_message>
update api sourcing of datetime and lat long
</commit_message>
<xml_diff>
--- a/eims-toi-transect/toi-transect.xlsx
+++ b/eims-toi-transect/toi-transect.xlsx
@@ -107,24 +107,9 @@
     <t>Oxygen-argon ratio divided by the reference ratio (oxygen-argon ratio in air minus 1, multiplied by 100)</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>Latitude of sample event</t>
-  </si>
-  <si>
     <t>degree</t>
   </si>
   <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>Longitude of sample event</t>
-  </si>
-  <si>
-    <t>depth_API_bottle_summary</t>
-  </si>
-  <si>
     <t>categorical</t>
   </si>
   <si>
@@ -149,19 +134,34 @@
     <t>PI-provided UTC date and time</t>
   </si>
   <si>
-    <t>Product UTC date and time from NES-LTER API</t>
-  </si>
-  <si>
     <t>depth_matlab</t>
   </si>
   <si>
     <t>PI-provided depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>Product depth of sample below sea surface from NES-LTER API</t>
-  </si>
-  <si>
     <t>Source of bottle sample whether from Niskin or underway</t>
+  </si>
+  <si>
+    <t>latitude_API</t>
+  </si>
+  <si>
+    <t>Latitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>longitude_API</t>
+  </si>
+  <si>
+    <t>Longitude of sample event provided by NES-LTER API</t>
+  </si>
+  <si>
+    <t>depth_API</t>
+  </si>
+  <si>
+    <t>Data product UTC date and time</t>
+  </si>
+  <si>
+    <t>Data product depth of sample below sea surface from CTD summary data in NES-LTER  API</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -553,10 +553,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -567,10 +567,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -581,30 +581,30 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -612,10 +612,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -660,10 +660,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -674,10 +674,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -716,10 +716,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -730,10 +730,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -744,10 +744,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
removed O2Ar & biosat from ncp output, wrote csvs for qc
</commit_message>
<xml_diff>
--- a/eims-toi-transect/toi-transect.xlsx
+++ b/eims-toi-transect/toi-transect.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8EB24B-68E2-4719-9AE0-EFE644427079}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -152,12 +147,6 @@
     <t xml:space="preserve">PI-provided depth of sample below sea surface. </t>
   </si>
   <si>
-    <t>Oxygen-17 composition of dissolved oxygen versus atmospheric O2</t>
-  </si>
-  <si>
-    <t>D17, triple isotopic composition of dissolved oxygen versus atmospheric O2</t>
-  </si>
-  <si>
     <t>d17O</t>
   </si>
   <si>
@@ -177,12 +166,18 @@
   </si>
   <si>
     <t>Data product depth of sample below sea surface, for underway samples depth of ship's intake, for Niskins from CTD summary data in NES-LTER  API. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-17 in dissolved oxygen (delta(17)O) in the water body by mass spectrometry</t>
+  </si>
+  <si>
+    <t>Triple isotopic composition of dissolved oxygen versus atmospheric O2, D17O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -192,10 +187,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <color rgb="FF1D1C1D"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -537,11 +533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -696,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -749,44 +745,44 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cap_Delta_17O unit, pkg 14 fixed methods & added plots
</commit_message>
<xml_diff>
--- a/eims-toi-transect/toi-transect.xlsx
+++ b/eims-toi-transect/toi-transect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8EB24B-68E2-4719-9AE0-EFE644427079}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D220F-74FC-4DC4-979D-24CBFAA60353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,12 +153,6 @@
     <t>d18O</t>
   </si>
   <si>
-    <t>permil</t>
-  </si>
-  <si>
-    <t>permeg</t>
-  </si>
-  <si>
     <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>Triple isotopic composition of dissolved oxygen versus atmospheric O2, D17O</t>
+  </si>
+  <si>
+    <t>perMeg</t>
+  </si>
+  <si>
+    <t>perMil</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -745,16 +745,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -762,13 +762,13 @@
         <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -776,13 +776,13 @@
         <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited methods, eims-toi abstract, and toi attribute
</commit_message>
<xml_diff>
--- a/eims-toi-transect/toi-transect.xlsx
+++ b/eims-toi-transect/toi-transect.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D220F-74FC-4DC4-979D-24CBFAA60353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FF1AE7-89EB-4F18-80F9-CA94C32AD656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>d18O</t>
   </si>
   <si>
-    <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry</t>
-  </si>
-  <si>
     <t>cap_Delta_17O</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>perMil</t>
+  </si>
+  <si>
+    <t>Enrichment of oxygen-18 in dissolved oxygen {18O in O2 CAS 14797-71-8} {delta(18)O} in the water body by mass spectrometry URI http://vocab.nerc.ac.uk/collection/P01/current/D18OMXDG/</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -745,16 +745,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -762,13 +762,13 @@
         <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -776,13 +776,13 @@
         <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>